<commit_message>
Update sub chi phí nguen lieu bc ke qua say
</commit_message>
<xml_diff>
--- a/Bao cao/Truong Son/bảng tổng hợp hiệu quả phân xưởng nguyên liệu.xlsx
+++ b/Bao cao/Truong Son/bảng tổng hợp hiệu quả phân xưởng nguyên liệu.xlsx
@@ -1713,8 +1713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:R68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="E39" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1724,6 +1724,7 @@
     <col min="4" max="4" width="19.85546875" customWidth="1"/>
     <col min="5" max="5" width="22.5703125" customWidth="1"/>
     <col min="6" max="6" width="16.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>